<commit_message>
Re-added MLR Round 13 forecasts with possiblity of a draw
</commit_message>
<xml_diff>
--- a/seasons/RugbyUnion/MajorLeagueRugby/2024/forecasts/ReportRound13.xlsx
+++ b/seasons/RugbyUnion/MajorLeagueRugby/2024/forecasts/ReportRound13.xlsx
@@ -91,6 +91,15 @@
     <t>95th Percentile Score</t>
   </si>
   <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>OGDC</t>
+  </si>
+  <si>
+    <t>Tukwila, WA</t>
+  </si>
+  <si>
     <t>MIA</t>
   </si>
   <si>
@@ -98,15 +107,6 @@
   </si>
   <si>
     <t>Fort Lauderdale, FL</t>
-  </si>
-  <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>OGDC</t>
-  </si>
-  <si>
-    <t>Tukwila, WA</t>
   </si>
   <si>
     <t>CHI</t>
@@ -148,6 +148,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF63B445"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC50A2A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF00B8F1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,22 +173,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC81A2E"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF63B445"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC50A2A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,6 +219,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF182A55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF092051"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF00AA"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -226,18 +238,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF031E41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF182A55"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF092051"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -700,11 +700,11 @@
         <v>1</v>
       </c>
       <c r="B3" s="11">
-        <v>0.6129771838805609</v>
+        <v>0.5655523591038107</v>
       </c>
       <c r="C3" s="11"/>
       <c r="E3" s="11">
-        <v>0.5655523591038107</v>
+        <v>0.6129771838805609</v>
       </c>
       <c r="F3" s="11"/>
       <c r="H3" s="11">
@@ -721,19 +721,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="11">
-        <v>0.8213386053523657</v>
+        <v>0.7837168331976709</v>
       </c>
       <c r="C4" s="11"/>
       <c r="E4" s="11">
-        <v>0.7931029026751412</v>
+        <v>0.8129771531562381</v>
       </c>
       <c r="F4" s="11"/>
       <c r="H4" s="11">
-        <v>0.988441569242526</v>
+        <v>0.987821882742574</v>
       </c>
       <c r="I4" s="11"/>
       <c r="K4" s="11">
-        <v>0.8860120901757036</v>
+        <v>0.8810120435361996</v>
       </c>
       <c r="L4" s="11"/>
     </row>
@@ -742,19 +742,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="10">
-        <v>50.34618253212805</v>
+        <v>44.32329038843105</v>
       </c>
       <c r="C5" s="10"/>
       <c r="E5" s="10">
-        <v>44.85412176200061</v>
+        <v>49.83364459009463</v>
       </c>
       <c r="F5" s="10"/>
       <c r="H5" s="10">
-        <v>60.63513861213237</v>
+        <v>60.59712445126553</v>
       </c>
       <c r="I5" s="10"/>
       <c r="K5" s="10">
-        <v>35.95821603224449</v>
+        <v>35.7552924387313</v>
       </c>
       <c r="L5" s="10"/>
     </row>
@@ -763,28 +763,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="12">
-        <v>0.2564478</v>
+        <v>0.7501118</v>
       </c>
       <c r="C6" s="12">
-        <v>0.7435522</v>
+        <v>0.2282502</v>
       </c>
       <c r="E6" s="12">
-        <v>0.7611618</v>
+        <v>0.2457324</v>
       </c>
       <c r="F6" s="12">
-        <v>0.2388382</v>
+        <v>0.7329896</v>
       </c>
       <c r="H6" s="12">
-        <v>0.5632071</v>
+        <v>0.5506952000000001</v>
       </c>
       <c r="I6" s="12">
-        <v>0.4367929</v>
+        <v>0.4242028</v>
       </c>
       <c r="K6" s="12">
-        <v>0.303905</v>
+        <v>0.2929386</v>
       </c>
       <c r="L6" s="12">
-        <v>0.696095</v>
+        <v>0.684266</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -792,28 +792,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="13">
-        <v>17.5781624</v>
+        <v>27.9814526</v>
       </c>
       <c r="C7" s="13">
-        <v>28.2168594</v>
+        <v>16.7662696</v>
       </c>
       <c r="E7" s="13">
-        <v>27.9912268</v>
+        <v>17.5807336</v>
       </c>
       <c r="F7" s="13">
-        <v>16.761435</v>
+        <v>28.2245148</v>
       </c>
       <c r="H7" s="13">
-        <v>27.4907498</v>
+        <v>27.4903616</v>
       </c>
       <c r="I7" s="13">
-        <v>24.5370446</v>
+        <v>24.5407482</v>
       </c>
       <c r="K7" s="13">
-        <v>19.9683864</v>
+        <v>19.9727256</v>
       </c>
       <c r="L7" s="13">
-        <v>28.5091706</v>
+        <v>28.4984666</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -821,16 +821,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="13">
+        <v>9</v>
+      </c>
+      <c r="C8" s="13">
         <v>3</v>
       </c>
-      <c r="C8" s="13">
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="13">
         <v>8</v>
-      </c>
-      <c r="E8" s="13">
-        <v>9</v>
-      </c>
-      <c r="F8" s="13">
-        <v>3</v>
       </c>
       <c r="H8" s="13">
         <v>7</v>
@@ -850,16 +850,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="13">
+        <v>13</v>
+      </c>
+      <c r="C9" s="13">
         <v>6</v>
       </c>
-      <c r="C9" s="13">
+      <c r="E9" s="13">
+        <v>6</v>
+      </c>
+      <c r="F9" s="13">
         <v>12</v>
-      </c>
-      <c r="E9" s="13">
-        <v>13</v>
-      </c>
-      <c r="F9" s="13">
-        <v>6</v>
       </c>
       <c r="H9" s="13">
         <v>12</v>
@@ -879,16 +879,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="13">
+        <v>15</v>
+      </c>
+      <c r="C10" s="13">
+        <v>7</v>
+      </c>
+      <c r="E10" s="13">
         <v>8</v>
       </c>
-      <c r="C10" s="13">
+      <c r="F10" s="13">
         <v>15</v>
-      </c>
-      <c r="E10" s="13">
-        <v>15</v>
-      </c>
-      <c r="F10" s="13">
-        <v>7</v>
       </c>
       <c r="H10" s="13">
         <v>14</v>
@@ -908,16 +908,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="13">
+        <v>17</v>
+      </c>
+      <c r="C11" s="13">
+        <v>8</v>
+      </c>
+      <c r="E11" s="13">
         <v>9</v>
       </c>
-      <c r="C11" s="13">
+      <c r="F11" s="13">
         <v>17</v>
-      </c>
-      <c r="E11" s="13">
-        <v>17</v>
-      </c>
-      <c r="F11" s="13">
-        <v>8</v>
       </c>
       <c r="H11" s="13">
         <v>15</v>
@@ -937,16 +937,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="13">
+        <v>19</v>
+      </c>
+      <c r="C12" s="13">
         <v>10</v>
       </c>
-      <c r="C12" s="13">
+      <c r="E12" s="13">
+        <v>10</v>
+      </c>
+      <c r="F12" s="13">
         <v>19</v>
-      </c>
-      <c r="E12" s="13">
-        <v>19</v>
-      </c>
-      <c r="F12" s="13">
-        <v>10</v>
       </c>
       <c r="H12" s="13">
         <v>18</v>
@@ -966,16 +966,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="13">
+        <v>20</v>
+      </c>
+      <c r="C13" s="13">
+        <v>11</v>
+      </c>
+      <c r="E13" s="13">
         <v>12</v>
       </c>
-      <c r="C13" s="13">
+      <c r="F13" s="13">
         <v>21</v>
-      </c>
-      <c r="E13" s="13">
-        <v>20</v>
-      </c>
-      <c r="F13" s="13">
-        <v>11</v>
       </c>
       <c r="H13" s="13">
         <v>20</v>
@@ -995,16 +995,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="13">
+        <v>22</v>
+      </c>
+      <c r="C14" s="13">
+        <v>12</v>
+      </c>
+      <c r="E14" s="13">
         <v>13</v>
       </c>
-      <c r="C14" s="13">
+      <c r="F14" s="13">
         <v>22</v>
-      </c>
-      <c r="E14" s="13">
-        <v>22</v>
-      </c>
-      <c r="F14" s="13">
-        <v>12</v>
       </c>
       <c r="H14" s="13">
         <v>21</v>
@@ -1024,16 +1024,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="13">
+        <v>24</v>
+      </c>
+      <c r="C15" s="13">
+        <v>13</v>
+      </c>
+      <c r="E15" s="13">
         <v>14</v>
       </c>
-      <c r="C15" s="13">
+      <c r="F15" s="13">
         <v>24</v>
-      </c>
-      <c r="E15" s="13">
-        <v>24</v>
-      </c>
-      <c r="F15" s="13">
-        <v>13</v>
       </c>
       <c r="H15" s="13">
         <v>23</v>
@@ -1053,16 +1053,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="13">
+        <v>25</v>
+      </c>
+      <c r="C16" s="13">
         <v>15</v>
       </c>
-      <c r="C16" s="13">
+      <c r="E16" s="13">
+        <v>15</v>
+      </c>
+      <c r="F16" s="13">
         <v>26</v>
-      </c>
-      <c r="E16" s="13">
-        <v>25</v>
-      </c>
-      <c r="F16" s="13">
-        <v>15</v>
       </c>
       <c r="H16" s="13">
         <v>24</v>
@@ -1082,16 +1082,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="13">
+        <v>27</v>
+      </c>
+      <c r="C17" s="13">
+        <v>16</v>
+      </c>
+      <c r="E17" s="13">
         <v>17</v>
       </c>
-      <c r="C17" s="13">
+      <c r="F17" s="13">
         <v>27</v>
-      </c>
-      <c r="E17" s="13">
-        <v>27</v>
-      </c>
-      <c r="F17" s="13">
-        <v>16</v>
       </c>
       <c r="H17" s="13">
         <v>26</v>
@@ -1111,16 +1111,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="13">
+        <v>29</v>
+      </c>
+      <c r="C18" s="13">
+        <v>17</v>
+      </c>
+      <c r="E18" s="13">
         <v>18</v>
       </c>
-      <c r="C18" s="13">
+      <c r="F18" s="13">
         <v>29</v>
-      </c>
-      <c r="E18" s="13">
-        <v>29</v>
-      </c>
-      <c r="F18" s="13">
-        <v>17</v>
       </c>
       <c r="H18" s="13">
         <v>28</v>
@@ -1140,16 +1140,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="13">
+        <v>30</v>
+      </c>
+      <c r="C19" s="13">
+        <v>18</v>
+      </c>
+      <c r="E19" s="13">
         <v>19</v>
       </c>
-      <c r="C19" s="13">
+      <c r="F19" s="13">
         <v>31</v>
-      </c>
-      <c r="E19" s="13">
-        <v>30</v>
-      </c>
-      <c r="F19" s="13">
-        <v>18</v>
       </c>
       <c r="H19" s="13">
         <v>29</v>
@@ -1169,16 +1169,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="13">
+        <v>32</v>
+      </c>
+      <c r="C20" s="13">
         <v>20</v>
       </c>
-      <c r="C20" s="13">
+      <c r="E20" s="13">
+        <v>20</v>
+      </c>
+      <c r="F20" s="13">
         <v>32</v>
-      </c>
-      <c r="E20" s="13">
-        <v>32</v>
-      </c>
-      <c r="F20" s="13">
-        <v>20</v>
       </c>
       <c r="H20" s="13">
         <v>31</v>
@@ -1198,16 +1198,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="13">
+        <v>34</v>
+      </c>
+      <c r="C21" s="13">
+        <v>21</v>
+      </c>
+      <c r="E21" s="13">
         <v>22</v>
       </c>
-      <c r="C21" s="13">
+      <c r="F21" s="13">
         <v>34</v>
-      </c>
-      <c r="E21" s="13">
-        <v>34</v>
-      </c>
-      <c r="F21" s="13">
-        <v>21</v>
       </c>
       <c r="H21" s="13">
         <v>34</v>
@@ -1227,16 +1227,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="13">
+        <v>36</v>
+      </c>
+      <c r="C22" s="13">
         <v>23</v>
       </c>
-      <c r="C22" s="13">
+      <c r="E22" s="13">
+        <v>23</v>
+      </c>
+      <c r="F22" s="13">
         <v>36</v>
-      </c>
-      <c r="E22" s="13">
-        <v>36</v>
-      </c>
-      <c r="F22" s="13">
-        <v>23</v>
       </c>
       <c r="H22" s="13">
         <v>36</v>
@@ -1256,16 +1256,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="13">
+        <v>38</v>
+      </c>
+      <c r="C23" s="13">
+        <v>24</v>
+      </c>
+      <c r="E23" s="13">
         <v>25</v>
       </c>
-      <c r="C23" s="13">
+      <c r="F23" s="13">
         <v>39</v>
-      </c>
-      <c r="E23" s="13">
-        <v>38</v>
-      </c>
-      <c r="F23" s="13">
-        <v>24</v>
       </c>
       <c r="H23" s="13">
         <v>38</v>
@@ -1285,16 +1285,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="13">
+        <v>41</v>
+      </c>
+      <c r="C24" s="13">
+        <v>27</v>
+      </c>
+      <c r="E24" s="13">
         <v>28</v>
       </c>
-      <c r="C24" s="13">
+      <c r="F24" s="13">
         <v>42</v>
-      </c>
-      <c r="E24" s="13">
-        <v>41</v>
-      </c>
-      <c r="F24" s="13">
-        <v>27</v>
       </c>
       <c r="H24" s="13">
         <v>41</v>
@@ -1314,16 +1314,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="13">
+        <v>45</v>
+      </c>
+      <c r="C25" s="13">
         <v>30</v>
       </c>
-      <c r="C25" s="13">
+      <c r="E25" s="13">
+        <v>30</v>
+      </c>
+      <c r="F25" s="13">
         <v>46</v>
-      </c>
-      <c r="E25" s="13">
-        <v>45</v>
-      </c>
-      <c r="F25" s="13">
-        <v>30</v>
       </c>
       <c r="H25" s="13">
         <v>45</v>
@@ -1343,16 +1343,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="13">
+        <v>51</v>
+      </c>
+      <c r="C26" s="13">
+        <v>34</v>
+      </c>
+      <c r="E26" s="13">
         <v>35</v>
       </c>
-      <c r="C26" s="13">
+      <c r="F26" s="13">
         <v>51</v>
-      </c>
-      <c r="E26" s="13">
-        <v>51</v>
-      </c>
-      <c r="F26" s="13">
-        <v>34</v>
       </c>
       <c r="H26" s="13">
         <v>51</v>

</xml_diff>